<commit_message>
Added Modeloramas set and implemented several minor template fixes
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template_3.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template_3.xlsx
@@ -33,6 +33,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$U$51</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -850,7 +851,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -943,11 +944,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1038,9 +1047,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>18360</xdr:colOff>
+      <xdr:colOff>18000</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1050,7 +1059,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6895080" cy="6352200"/>
+          <a:ext cx="6809040" cy="6351840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1087,32 +1096,32 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N51" activeCellId="0" sqref="N51"/>
+      <selection pane="bottomLeft" activeCell="Q53" activeCellId="0" sqref="Q53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="79.9132653061225"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="94.765306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="78.9693877551021"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="93.6836734693878"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3877,60 +3886,61 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="23" t="s">
+      <c r="E51" s="23"/>
+      <c r="F51" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="G51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M51" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N51" s="8" t="n">
+      <c r="G51" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K51" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L51" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M51" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="N51" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="O51" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="P51" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="R51" s="8" t="s">
+      <c r="O51" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="P51" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q51" s="25"/>
+      <c r="R51" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="S51" s="8" t="s">
+      <c r="S51" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="T51" s="22" t="s">
+      <c r="T51" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="U51" s="8" t="s">
+      <c r="U51" s="23" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3961,11 +3971,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.2397959183674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.7040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3994,7 +4004,7 @@
       <c r="B4" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="27" t="s">
         <v>173</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -4092,7 +4102,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4118,8 +4128,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4166,7 +4176,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>